<commit_message>
SVN (res) commit #2306 by scriswellwsf       ruleset mods w/ cool roof updates for 2022 code (tic $1302)
</commit_message>
<xml_diff>
--- a/RulesetDev/Rulesets/CA Res/Rules/T24RClimateZoneCodeBaselines.xlsx
+++ b/RulesetDev/Rulesets/CA Res/Rules/T24RClimateZoneCodeBaselines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\svn-CEC\SF_CBECC-Res\trunk\RulesetDev\Rulesets\CA Res\Rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4775BF9-BB3E-4266-B93D-1AF3E135781D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7575A7D-86F0-4C2C-B0FA-7186571AAF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2490" windowWidth="20640" windowHeight="12015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="0" windowWidth="24060" windowHeight="14310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T24RClimateZoneCodeBaselines" sheetId="1" r:id="rId1"/>
@@ -3335,13 +3335,13 @@
     <t>AltLowRoofRiseAboveDeckIns - presriptive reqs for Altered, LowRoofRise (&lt; 2:12) roof above deck insulation</t>
   </si>
   <si>
-    <t>12/13/22 - SAC - added new col: AltLowRoofRiseAboveDeckIns - presriptive reqs for Altered, LowRoofRise (&lt; 2:12) roof above deck insulation (tic #1302)</t>
-  </si>
-  <si>
     <t>added - SAC 12/13/22 (tic #1302)</t>
   </si>
   <si>
     <t>R14 Sheathing</t>
+  </si>
+  <si>
+    <t>12/13/22 - SAC - added new col: AltLowRoofRiseAboveDeckIns - prescriptive reqs for Altered, LowRoofRise (&lt; 2:12) roof above deck insulation -and- revised SteepRoofReflect &amp; FlatRoofReflect for '22+ code vintages (tic #1302)</t>
   </si>
 </sst>
 </file>
@@ -4647,8 +4647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EY396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AM355" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AT372" sqref="AT372"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4756,7 +4756,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5962,7 +5962,7 @@
         <v>339</v>
       </c>
       <c r="P101" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y101" t="s">
         <v>9</v>
@@ -52585,7 +52585,7 @@
         <v>116</v>
       </c>
       <c r="AU331" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV331" s="3" t="s">
         <v>116</v>
@@ -52808,7 +52808,7 @@
         <v>116</v>
       </c>
       <c r="AU332" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV332" s="3" t="s">
         <v>116</v>
@@ -53258,17 +53258,17 @@
       <c r="AQ334" s="27">
         <v>0</v>
       </c>
-      <c r="AR334" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="AS334" s="27">
-        <v>0.1</v>
+      <c r="AR334" s="100">
+        <v>0.2</v>
+      </c>
+      <c r="AS334" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT334" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU334" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV334" s="3" t="s">
         <v>204</v>
@@ -53721,8 +53721,8 @@
       <c r="AR336" s="27">
         <v>0.1</v>
       </c>
-      <c r="AS336" s="27">
-        <v>0.1</v>
+      <c r="AS336" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT336" s="3" t="s">
         <v>116</v>
@@ -53950,8 +53950,8 @@
       <c r="AR337" s="27">
         <v>0.1</v>
       </c>
-      <c r="AS337" s="27">
-        <v>0.1</v>
+      <c r="AS337" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT337" s="3" t="s">
         <v>116</v>
@@ -54176,17 +54176,17 @@
       <c r="AQ338" s="27">
         <v>0</v>
       </c>
-      <c r="AR338" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="AS338" s="27">
-        <v>0.1</v>
+      <c r="AR338" s="100">
+        <v>0.2</v>
+      </c>
+      <c r="AS338" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT338" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU338" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV338" s="3" t="s">
         <v>204</v>
@@ -54405,17 +54405,17 @@
       <c r="AQ339" s="27">
         <v>0</v>
       </c>
-      <c r="AR339" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="AS339" s="27">
-        <v>0.1</v>
+      <c r="AR339" s="100">
+        <v>0.2</v>
+      </c>
+      <c r="AS339" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT339" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU339" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV339" s="3" t="s">
         <v>204</v>
@@ -54638,14 +54638,14 @@
       <c r="AR340" s="27">
         <v>0.2</v>
       </c>
-      <c r="AS340" s="27">
-        <v>0.1</v>
+      <c r="AS340" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT340" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU340" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV340" s="3" t="s">
         <v>204</v>
@@ -54868,14 +54868,14 @@
       <c r="AR341" s="27">
         <v>0.2</v>
       </c>
-      <c r="AS341" s="27">
-        <v>0.1</v>
+      <c r="AS341" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT341" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU341" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV341" s="3" t="s">
         <v>204</v>
@@ -55098,14 +55098,14 @@
       <c r="AR342" s="27">
         <v>0.2</v>
       </c>
-      <c r="AS342" s="27">
-        <v>0.1</v>
+      <c r="AS342" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT342" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU342" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV342" s="3" t="s">
         <v>204</v>
@@ -55335,7 +55335,7 @@
         <v>116</v>
       </c>
       <c r="AU343" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV343" s="3" t="s">
         <v>204</v>
@@ -55558,14 +55558,14 @@
       <c r="AR344" s="27">
         <v>0.2</v>
       </c>
-      <c r="AS344" s="27">
-        <v>0.1</v>
+      <c r="AS344" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT344" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU344" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV344" s="3" t="s">
         <v>204</v>
@@ -55795,7 +55795,7 @@
         <v>116</v>
       </c>
       <c r="AU345" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV345" s="3" t="s">
         <v>204</v>
@@ -56025,7 +56025,7 @@
         <v>116</v>
       </c>
       <c r="AU346" s="108" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV346" s="84" t="s">
         <v>204</v>
@@ -60241,7 +60241,7 @@
         <v>116</v>
       </c>
       <c r="AU364" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV364" s="3" t="s">
         <v>116</v>
@@ -60464,7 +60464,7 @@
         <v>116</v>
       </c>
       <c r="AU365" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV365" s="3" t="s">
         <v>116</v>
@@ -60914,17 +60914,17 @@
       <c r="AQ367" s="27">
         <v>0</v>
       </c>
-      <c r="AR367" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="AS367" s="27">
-        <v>0.1</v>
+      <c r="AR367" s="100">
+        <v>0.2</v>
+      </c>
+      <c r="AS367" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT367" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU367" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV367" s="3" t="s">
         <v>204</v>
@@ -61377,8 +61377,8 @@
       <c r="AR369" s="27">
         <v>0.1</v>
       </c>
-      <c r="AS369" s="27">
-        <v>0.1</v>
+      <c r="AS369" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT369" s="3" t="s">
         <v>116</v>
@@ -61606,8 +61606,8 @@
       <c r="AR370" s="27">
         <v>0.1</v>
       </c>
-      <c r="AS370" s="27">
-        <v>0.1</v>
+      <c r="AS370" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT370" s="3" t="s">
         <v>116</v>
@@ -61832,17 +61832,17 @@
       <c r="AQ371" s="27">
         <v>0</v>
       </c>
-      <c r="AR371" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="AS371" s="27">
-        <v>0.1</v>
+      <c r="AR371" s="100">
+        <v>0.2</v>
+      </c>
+      <c r="AS371" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT371" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU371" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV371" s="3" t="s">
         <v>204</v>
@@ -62061,17 +62061,17 @@
       <c r="AQ372" s="27">
         <v>0</v>
       </c>
-      <c r="AR372" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="AS372" s="27">
-        <v>0.1</v>
+      <c r="AR372" s="100">
+        <v>0.2</v>
+      </c>
+      <c r="AS372" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT372" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU372" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV372" s="3" t="s">
         <v>204</v>
@@ -62294,14 +62294,14 @@
       <c r="AR373" s="27">
         <v>0.2</v>
       </c>
-      <c r="AS373" s="27">
-        <v>0.1</v>
+      <c r="AS373" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT373" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU373" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV373" s="3" t="s">
         <v>204</v>
@@ -62524,14 +62524,14 @@
       <c r="AR374" s="27">
         <v>0.2</v>
       </c>
-      <c r="AS374" s="27">
-        <v>0.1</v>
+      <c r="AS374" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT374" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU374" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV374" s="3" t="s">
         <v>204</v>
@@ -62754,14 +62754,14 @@
       <c r="AR375" s="27">
         <v>0.2</v>
       </c>
-      <c r="AS375" s="27">
-        <v>0.1</v>
+      <c r="AS375" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT375" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU375" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV375" s="3" t="s">
         <v>204</v>
@@ -62991,7 +62991,7 @@
         <v>116</v>
       </c>
       <c r="AU376" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV376" s="3" t="s">
         <v>204</v>
@@ -63214,14 +63214,14 @@
       <c r="AR377" s="27">
         <v>0.2</v>
       </c>
-      <c r="AS377" s="27">
-        <v>0.1</v>
+      <c r="AS377" s="100">
+        <v>0.63</v>
       </c>
       <c r="AT377" s="3" t="s">
         <v>116</v>
       </c>
       <c r="AU377" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV377" s="3" t="s">
         <v>204</v>
@@ -63451,7 +63451,7 @@
         <v>116</v>
       </c>
       <c r="AU378" s="99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV378" s="3" t="s">
         <v>204</v>
@@ -63681,7 +63681,7 @@
         <v>116</v>
       </c>
       <c r="AU379" s="108" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV379" s="84" t="s">
         <v>204</v>

</xml_diff>